<commit_message>
add results for Genetic Algorithms
</commit_message>
<xml_diff>
--- a/memoria/resources/Tablas_MDD_2021-22.xlsx
+++ b/memoria/resources/Tablas_MDD_2021-22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/MH/memoria/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6661C7C-AC10-324E-8717-0F15C9F03AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29C5524-B505-254F-B8F9-76EC43C11F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-80" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2021-22" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2021-22'!$H$4:$H$53</definedName>
-    <definedName name="_xlchart.v1.0" hidden="1">'2021-22'!$G$4:$G$53</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'2021-22'!$O$4:$O$53</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'2021-22'!$W$4:$W$53</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'2021-22'!$AE$4:$AE$53</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'2021-22'!$AM$4:$AM$53</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'2021-22'!$AU$4:$AU$53</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'2021-22'!$BC$4:$BC$53</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'2021-22'!$G$4:$G$53</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'2021-22'!$O$4:$O$53</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'2021-22'!$W$4:$W$53</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'2021-22'!$G$4:$G$53</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'2021-22'!$O$4:$O$53</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'2021-22'!$W$4:$W$53</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase" localSheetId="0">'2021-22'!$H$4:$H$53</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -41,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="71">
   <si>
     <t>Nº casos:</t>
   </si>
@@ -234,6 +241,27 @@
   <si>
     <t>Algoritmo Búsqueda Local</t>
   </si>
+  <si>
+    <t>Algoritmo AGG-uniforme</t>
+  </si>
+  <si>
+    <t>Algoritmo AGG-position</t>
+  </si>
+  <si>
+    <t>semilla 1</t>
+  </si>
+  <si>
+    <t>semilla 1,2,3,4,5</t>
+  </si>
+  <si>
+    <t>semilla 2</t>
+  </si>
+  <si>
+    <t>Algoritmo AGE-uniforme</t>
+  </si>
+  <si>
+    <t>Algoritmo AGE-posicion</t>
+  </si>
 </sst>
 </file>
 
@@ -392,7 +420,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
@@ -484,12 +512,108 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="16"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="16"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="16"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="16"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="16"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="16"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -621,17 +745,37 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
+        <cx:f>_xlchart.v1.6</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="3">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.0</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="4">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.1</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="5">
+      <cx:numDim type="val">
         <cx:f>_xlchart.v1.2</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="6">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -672,6 +816,50 @@
             </cx:txData>
           </cx:tx>
           <cx:dataId val="2"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000000-D01A-BF43-80AD-3C2244F3DAB4}">
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Algoritmo AGG-uniforme</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="3"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000001-D01A-BF43-80AD-3C2244F3DAB4}">
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Algoritmo AGG-posicion</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="4"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000002-D01A-BF43-80AD-3C2244F3DAB4}">
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Algoritmo AGE-uniforme</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="5"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000003-D01A-BF43-80AD-3C2244F3DAB4}">
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Algoritmo AGE-posicion</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="6"/>
           <cx:layoutPr>
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
@@ -1686,10 +1874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB53"/>
+  <dimension ref="A1:BH55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4:Y53"/>
+    <sheetView tabSelected="1" topLeftCell="AK1" zoomScale="61" zoomScaleNormal="61" workbookViewId="0">
+      <selection activeCell="BK21" sqref="BK21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1706,7 +1894,7 @@
     <col min="22" max="22" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:60" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1726,38 +1914,62 @@
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:28" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:60" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
       <c r="J2" s="7"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
-      <c r="N2" s="36" t="s">
+      <c r="N2" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="36"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
       <c r="R2" s="7"/>
       <c r="S2" s="8"/>
       <c r="T2" s="8"/>
-      <c r="V2" s="36" t="s">
+      <c r="V2" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="W2" s="36"/>
-      <c r="X2" s="36"/>
-      <c r="Y2" s="36"/>
-    </row>
-    <row r="3" spans="1:28" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="W2" s="37"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="37"/>
+      <c r="AD2" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE2" s="37"/>
+      <c r="AF2" s="37"/>
+      <c r="AG2" s="37"/>
+      <c r="AL2" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="AM2" s="37"/>
+      <c r="AN2" s="37"/>
+      <c r="AO2" s="37"/>
+      <c r="AT2" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="AU2" s="37"/>
+      <c r="AV2" s="37"/>
+      <c r="AW2" s="37"/>
+      <c r="BB2" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="BC2" s="37"/>
+      <c r="BD2" s="37"/>
+      <c r="BE2" s="37"/>
+    </row>
+    <row r="3" spans="1:60" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
@@ -1813,8 +2025,56 @@
       <c r="Y3" s="14" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:28" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF3" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="AL3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN3" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="AO3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="AT3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="AU3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="AV3" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="AW3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="BB3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="BC3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="BD3" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="BE3" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:60" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>8</v>
       </c>
@@ -1873,8 +2133,60 @@
       <c r="Y4" s="22">
         <v>1.4810800000000001E-5</v>
       </c>
-    </row>
-    <row r="5" spans="1:28" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="21">
+        <f>(AE4-$D4)</f>
+        <v>0</v>
+      </c>
+      <c r="AG4" s="22">
+        <v>6.0821399999999998E-2</v>
+      </c>
+      <c r="AL4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="AM4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="21">
+        <f>(AM4-$D4)</f>
+        <v>0</v>
+      </c>
+      <c r="AO4" s="22">
+        <v>6.6202800000000006E-2</v>
+      </c>
+      <c r="AT4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AV4" s="21">
+        <f>(AU4-$D4)</f>
+        <v>0</v>
+      </c>
+      <c r="AW4" s="22">
+        <v>6.9199899999999995E-2</v>
+      </c>
+      <c r="BB4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="BC4" s="20">
+        <v>0</v>
+      </c>
+      <c r="BD4" s="21">
+        <f>(BC4-$D4)</f>
+        <v>0</v>
+      </c>
+      <c r="BE4" s="22">
+        <v>7.3221599999999998E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:60" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>9</v>
       </c>
@@ -1933,8 +2245,60 @@
       <c r="Y5" s="22">
         <v>1.47072E-5</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD5" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="21">
+        <f>(AE5-$D5)</f>
+        <v>0</v>
+      </c>
+      <c r="AG5" s="22">
+        <v>6.0160499999999999E-2</v>
+      </c>
+      <c r="AL5" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="AM5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AN5" s="21">
+        <f>(AM5-$D5)</f>
+        <v>0</v>
+      </c>
+      <c r="AO5" s="22">
+        <v>6.1093799999999997E-2</v>
+      </c>
+      <c r="AT5" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="AU5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AV5" s="21">
+        <f>(AU5-$D5)</f>
+        <v>0</v>
+      </c>
+      <c r="AW5" s="22">
+        <v>6.8857500000000002E-2</v>
+      </c>
+      <c r="BB5" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="BC5" s="20">
+        <v>0</v>
+      </c>
+      <c r="BD5" s="21">
+        <f>(BC5-$D5)</f>
+        <v>0</v>
+      </c>
+      <c r="BE5" s="22">
+        <v>7.2994299999999998E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:60" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>10</v>
       </c>
@@ -2010,8 +2374,88 @@
         <f>SUM(X4:X53)/$B$1</f>
         <v>94.790220080000054</v>
       </c>
-    </row>
-    <row r="7" spans="1:28" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD6" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="21">
+        <f>(AE6-$D6)</f>
+        <v>0</v>
+      </c>
+      <c r="AG6" s="22">
+        <v>6.01253E-2</v>
+      </c>
+      <c r="AI6" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ6" s="24">
+        <f>SUM(AF4:AF53)/$B$1</f>
+        <v>77.377226600000057</v>
+      </c>
+      <c r="AL6" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AN6" s="21">
+        <f>(AM6-$D6)</f>
+        <v>0</v>
+      </c>
+      <c r="AO6" s="22">
+        <v>5.8037199999999997E-2</v>
+      </c>
+      <c r="AQ6" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="AR6" s="24">
+        <f>SUM(AN4:AN53)/$B$1</f>
+        <v>97.221302000000051</v>
+      </c>
+      <c r="AT6" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="AU6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AV6" s="21">
+        <f>(AU6-$D6)</f>
+        <v>0</v>
+      </c>
+      <c r="AW6" s="22">
+        <v>6.9070199999999998E-2</v>
+      </c>
+      <c r="AY6" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="AZ6" s="24">
+        <f>SUM(AV4:AV53)/$B$1</f>
+        <v>29.876160800000051</v>
+      </c>
+      <c r="BB6" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="BC6" s="20">
+        <v>0</v>
+      </c>
+      <c r="BD6" s="21">
+        <f>(BC6-$D6)</f>
+        <v>0</v>
+      </c>
+      <c r="BE6" s="22">
+        <v>7.3031700000000005E-2</v>
+      </c>
+      <c r="BG6" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="BH6" s="24">
+        <f>SUM(BD4:BD53)/$B$1</f>
+        <v>42.145252800000051</v>
+      </c>
+    </row>
+    <row r="7" spans="1:60" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>12</v>
       </c>
@@ -2087,8 +2531,88 @@
         <f>SUM(Y4:Y53)/$B$1</f>
         <v>1.5571758132000003E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD7" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="21">
+        <f>(AE7-$D7)</f>
+        <v>0</v>
+      </c>
+      <c r="AG7" s="22">
+        <v>6.1005499999999997E-2</v>
+      </c>
+      <c r="AI7" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ7" s="25">
+        <f>SUM(AG4:AG53)/$B$1</f>
+        <v>5.3775699280000007</v>
+      </c>
+      <c r="AL7" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AN7" s="21">
+        <f>(AM7-$D7)</f>
+        <v>0</v>
+      </c>
+      <c r="AO7" s="22">
+        <v>6.4510999999999999E-2</v>
+      </c>
+      <c r="AQ7" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="AR7" s="25">
+        <f>SUM(AO4:AO53)/$B$1</f>
+        <v>1.1049505740000001</v>
+      </c>
+      <c r="AT7" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AV7" s="21">
+        <f>(AU7-$D7)</f>
+        <v>0</v>
+      </c>
+      <c r="AW7" s="22">
+        <v>6.9793800000000003E-2</v>
+      </c>
+      <c r="AY7" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="AZ7" s="25">
+        <f>SUM(AW4:AW53)/$B$1</f>
+        <v>8.8108092439999979</v>
+      </c>
+      <c r="BB7" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="BC7" s="20">
+        <v>0</v>
+      </c>
+      <c r="BD7" s="21">
+        <f>(BC7-$D7)</f>
+        <v>0</v>
+      </c>
+      <c r="BE7" s="22">
+        <v>7.4018399999999998E-2</v>
+      </c>
+      <c r="BG7" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="BH7" s="25">
+        <f>SUM(BE4:BE53)/$B$1</f>
+        <v>0.95357937200000009</v>
+      </c>
+    </row>
+    <row r="8" spans="1:60" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>14</v>
       </c>
@@ -2147,8 +2671,60 @@
       <c r="Y8" s="22">
         <v>1.42838E-5</v>
       </c>
-    </row>
-    <row r="9" spans="1:28" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD8" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="21">
+        <f>(AE8-$D8)</f>
+        <v>0</v>
+      </c>
+      <c r="AG8" s="22">
+        <v>6.1448700000000002E-2</v>
+      </c>
+      <c r="AL8" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="AM8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AN8" s="21">
+        <f>(AM8-$D8)</f>
+        <v>0</v>
+      </c>
+      <c r="AO8" s="22">
+        <v>6.2091899999999998E-2</v>
+      </c>
+      <c r="AT8" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="AU8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AV8" s="21">
+        <f>(AU8-$D8)</f>
+        <v>0</v>
+      </c>
+      <c r="AW8" s="22">
+        <v>6.9232799999999997E-2</v>
+      </c>
+      <c r="BB8" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="BC8" s="20">
+        <v>0</v>
+      </c>
+      <c r="BD8" s="21">
+        <f>(BC8-$D8)</f>
+        <v>0</v>
+      </c>
+      <c r="BE8" s="22">
+        <v>7.3707599999999998E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:60" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>15</v>
       </c>
@@ -2207,8 +2783,60 @@
       <c r="Y9" s="22">
         <v>2.4675400000000002E-4</v>
       </c>
-    </row>
-    <row r="10" spans="1:28" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD9" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE9" s="20">
+        <v>13.4793</v>
+      </c>
+      <c r="AF9" s="21">
+        <f>(AE9-$D9)</f>
+        <v>0.76134000000030078</v>
+      </c>
+      <c r="AG9" s="22">
+        <v>0.29059200000000002</v>
+      </c>
+      <c r="AL9" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="AM9" s="20">
+        <v>13.4793</v>
+      </c>
+      <c r="AN9" s="21">
+        <f>(AM9-$D9)</f>
+        <v>0.76134000000030078</v>
+      </c>
+      <c r="AO9" s="22">
+        <v>0.22487699999999999</v>
+      </c>
+      <c r="AT9" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="AU9" s="20">
+        <v>27.352</v>
+      </c>
+      <c r="AV9" s="21">
+        <f>(AU9-$D9)</f>
+        <v>14.634040000000301</v>
+      </c>
+      <c r="AW9" s="22">
+        <v>0.20604</v>
+      </c>
+      <c r="BB9" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="BC9" s="20">
+        <v>38.9437</v>
+      </c>
+      <c r="BD9" s="21">
+        <f>(BC9-$D9)</f>
+        <v>26.2257400000003</v>
+      </c>
+      <c r="BE9" s="22">
+        <v>0.20511599999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:60" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>16</v>
       </c>
@@ -2267,8 +2895,60 @@
       <c r="Y10" s="22">
         <v>2.0526499999999999E-4</v>
       </c>
-    </row>
-    <row r="11" spans="1:28" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD10" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE10" s="20">
+        <v>14.098800000000001</v>
+      </c>
+      <c r="AF10" s="21">
+        <f>(AE10-$D10)</f>
+        <v>5.0000000300087777E-5</v>
+      </c>
+      <c r="AG10" s="22">
+        <v>0.28697600000000001</v>
+      </c>
+      <c r="AL10" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="AM10" s="20">
+        <v>16.742999999999999</v>
+      </c>
+      <c r="AN10" s="21">
+        <f>(AM10-$D10)</f>
+        <v>2.644250000000298</v>
+      </c>
+      <c r="AO10" s="22">
+        <v>0.23469200000000001</v>
+      </c>
+      <c r="AT10" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="AU10" s="20">
+        <v>22.354099999999999</v>
+      </c>
+      <c r="AV10" s="21">
+        <f>(AU10-$D10)</f>
+        <v>8.2553500000002984</v>
+      </c>
+      <c r="AW10" s="22">
+        <v>0.20652200000000001</v>
+      </c>
+      <c r="BB10" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="BC10" s="20">
+        <v>22.264900000000001</v>
+      </c>
+      <c r="BD10" s="21">
+        <f>(BC10-$D10)</f>
+        <v>8.1661500000003002</v>
+      </c>
+      <c r="BE10" s="22">
+        <v>0.205261</v>
+      </c>
+    </row>
+    <row r="11" spans="1:60" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>17</v>
       </c>
@@ -2327,8 +3007,60 @@
       <c r="Y11" s="22">
         <v>2.8544900000000001E-4</v>
       </c>
-    </row>
-    <row r="12" spans="1:28" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD11" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE11" s="20">
+        <v>16.761199999999999</v>
+      </c>
+      <c r="AF11" s="21">
+        <f>(AE11-$D11)</f>
+        <v>1.0000000198573389E-5</v>
+      </c>
+      <c r="AG11" s="22">
+        <v>0.27321000000000001</v>
+      </c>
+      <c r="AL11" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="AM11" s="20">
+        <v>21.826499999999999</v>
+      </c>
+      <c r="AN11" s="21">
+        <f>(AM11-$D11)</f>
+        <v>5.0653100000001992</v>
+      </c>
+      <c r="AO11" s="22">
+        <v>0.25509300000000001</v>
+      </c>
+      <c r="AT11" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="AU11" s="20">
+        <v>21.826499999999999</v>
+      </c>
+      <c r="AV11" s="21">
+        <f>(AU11-$D11)</f>
+        <v>5.0653100000001992</v>
+      </c>
+      <c r="AW11" s="22">
+        <v>0.20524800000000001</v>
+      </c>
+      <c r="BB11" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="BC11" s="20">
+        <v>29.119399999999999</v>
+      </c>
+      <c r="BD11" s="21">
+        <f>(BC11-$D11)</f>
+        <v>12.358210000000199</v>
+      </c>
+      <c r="BE11" s="22">
+        <v>0.205599</v>
+      </c>
+    </row>
+    <row r="12" spans="1:60" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>18</v>
       </c>
@@ -2387,8 +3119,60 @@
       <c r="Y12" s="22">
         <v>2.3288599999999999E-4</v>
       </c>
-    </row>
-    <row r="13" spans="1:28" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE12" s="20">
+        <v>21.739100000000001</v>
+      </c>
+      <c r="AF12" s="21">
+        <f>(AE12-$D12)</f>
+        <v>4.6698900000001018</v>
+      </c>
+      <c r="AG12" s="22">
+        <v>0.27059499999999997</v>
+      </c>
+      <c r="AL12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="AM12" s="20">
+        <v>17.069199999999999</v>
+      </c>
+      <c r="AN12" s="21">
+        <f>(AM12-$D12)</f>
+        <v>-9.9999999001454398E-6</v>
+      </c>
+      <c r="AO12" s="22">
+        <v>0.26447900000000002</v>
+      </c>
+      <c r="AT12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="AU12" s="20">
+        <v>17.069199999999999</v>
+      </c>
+      <c r="AV12" s="21">
+        <f>(AU12-$D12)</f>
+        <v>-9.9999999001454398E-6</v>
+      </c>
+      <c r="AW12" s="22">
+        <v>0.221641</v>
+      </c>
+      <c r="BB12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="BC12" s="20">
+        <v>17.069199999999999</v>
+      </c>
+      <c r="BD12" s="21">
+        <f>(BC12-$D12)</f>
+        <v>-9.9999999001454398E-6</v>
+      </c>
+      <c r="BE12" s="22">
+        <v>0.222576</v>
+      </c>
+    </row>
+    <row r="13" spans="1:60" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>19</v>
       </c>
@@ -2447,8 +3231,60 @@
       <c r="Y13" s="22">
         <v>2.00342E-4</v>
       </c>
-    </row>
-    <row r="14" spans="1:28" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD13" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE13" s="20">
+        <v>26.238</v>
+      </c>
+      <c r="AF13" s="21">
+        <f>(AE13-$D13)</f>
+        <v>2.9727700000001001</v>
+      </c>
+      <c r="AG13" s="22">
+        <v>0.30552200000000002</v>
+      </c>
+      <c r="AL13" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM13" s="20">
+        <v>26.238</v>
+      </c>
+      <c r="AN13" s="21">
+        <f>(AM13-$D13)</f>
+        <v>2.9727700000001001</v>
+      </c>
+      <c r="AO13" s="22">
+        <v>0.24903900000000001</v>
+      </c>
+      <c r="AT13" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="AU13" s="20">
+        <v>31.435600000000001</v>
+      </c>
+      <c r="AV13" s="21">
+        <f>(AU13-$D13)</f>
+        <v>8.1703700000001014</v>
+      </c>
+      <c r="AW13" s="22">
+        <v>0.227964</v>
+      </c>
+      <c r="BB13" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="BC13" s="20">
+        <v>28.128699999999998</v>
+      </c>
+      <c r="BD13" s="21">
+        <f>(BC13-$D13)</f>
+        <v>4.863470000000099</v>
+      </c>
+      <c r="BE13" s="22">
+        <v>0.223662</v>
+      </c>
+    </row>
+    <row r="14" spans="1:60" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>20</v>
       </c>
@@ -2507,8 +3343,60 @@
       <c r="Y14" s="22">
         <v>2.2503200000000001E-4</v>
       </c>
-    </row>
-    <row r="15" spans="1:28" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD14" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE14" s="20">
+        <v>1.9260900000000001</v>
+      </c>
+      <c r="AF14" s="21">
+        <f>(AE14-$D14)</f>
+        <v>-1.0000000019827482E-5</v>
+      </c>
+      <c r="AG14" s="22">
+        <v>0.20275799999999999</v>
+      </c>
+      <c r="AL14" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="AM14" s="20">
+        <v>1.9260900000000001</v>
+      </c>
+      <c r="AN14" s="21">
+        <f>(AM14-$D14)</f>
+        <v>-1.0000000019827482E-5</v>
+      </c>
+      <c r="AO14" s="22">
+        <v>0.162693</v>
+      </c>
+      <c r="AT14" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="AU14" s="20">
+        <v>11.4673</v>
+      </c>
+      <c r="AV14" s="21">
+        <f>(AU14-$D14)</f>
+        <v>9.5411999999999804</v>
+      </c>
+      <c r="AW14" s="22">
+        <v>0.14891299999999999</v>
+      </c>
+      <c r="BB14" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="BC14" s="20">
+        <v>11.586</v>
+      </c>
+      <c r="BD14" s="21">
+        <f>(BC14-$D14)</f>
+        <v>9.6598999999999808</v>
+      </c>
+      <c r="BE14" s="22">
+        <v>0.150537</v>
+      </c>
+    </row>
+    <row r="15" spans="1:60" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>21</v>
       </c>
@@ -2567,8 +3455,60 @@
       <c r="Y15" s="22">
         <v>2.6800700000000001E-4</v>
       </c>
-    </row>
-    <row r="16" spans="1:28" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD15" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE15" s="20">
+        <v>2.9138199999999999</v>
+      </c>
+      <c r="AF15" s="21">
+        <f>(AE15-$D15)</f>
+        <v>0.79277999999988991</v>
+      </c>
+      <c r="AG15" s="22">
+        <v>0.207368</v>
+      </c>
+      <c r="AL15" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM15" s="20">
+        <v>6.8786800000000001</v>
+      </c>
+      <c r="AN15" s="21">
+        <f>(AM15-$D15)</f>
+        <v>4.7576399999998902</v>
+      </c>
+      <c r="AO15" s="22">
+        <v>0.17338500000000001</v>
+      </c>
+      <c r="AT15" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="AU15" s="20">
+        <v>8.2328899999999994</v>
+      </c>
+      <c r="AV15" s="21">
+        <f>(AU15-$D15)</f>
+        <v>6.1118499999998894</v>
+      </c>
+      <c r="AW15" s="22">
+        <v>0.147392</v>
+      </c>
+      <c r="BB15" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="BC15" s="20">
+        <v>8.52576</v>
+      </c>
+      <c r="BD15" s="21">
+        <f>(BC15-$D15)</f>
+        <v>6.4047199999998901</v>
+      </c>
+      <c r="BE15" s="22">
+        <v>0.14832500000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:60" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>22</v>
       </c>
@@ -2627,8 +3567,60 @@
       <c r="Y16" s="22">
         <v>3.06812E-4</v>
       </c>
-    </row>
-    <row r="17" spans="1:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD16" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE16" s="20">
+        <v>3.4638499999999999</v>
+      </c>
+      <c r="AF16" s="21">
+        <f>(AE16-$D16)</f>
+        <v>1.1015400000000199</v>
+      </c>
+      <c r="AG16" s="22">
+        <v>0.202296</v>
+      </c>
+      <c r="AL16" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM16" s="20">
+        <v>9.7211599999999994</v>
+      </c>
+      <c r="AN16" s="21">
+        <f>(AM16-$D16)</f>
+        <v>7.3588500000000199</v>
+      </c>
+      <c r="AO16" s="22">
+        <v>0.159223</v>
+      </c>
+      <c r="AT16" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="AU16" s="20">
+        <v>9.5356000000000005</v>
+      </c>
+      <c r="AV16" s="21">
+        <f>(AU16-$D16)</f>
+        <v>7.173290000000021</v>
+      </c>
+      <c r="AW16" s="22">
+        <v>0.14518300000000001</v>
+      </c>
+      <c r="BB16" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="BC16" s="20">
+        <v>17.350300000000001</v>
+      </c>
+      <c r="BD16" s="21">
+        <f>(BC16-$D16)</f>
+        <v>14.987990000000021</v>
+      </c>
+      <c r="BE16" s="22">
+        <v>0.148316</v>
+      </c>
+    </row>
+    <row r="17" spans="1:57" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>23</v>
       </c>
@@ -2687,8 +3679,60 @@
       <c r="Y17" s="22">
         <v>2.2628399999999999E-4</v>
       </c>
-    </row>
-    <row r="18" spans="1:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD17" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE17" s="20">
+        <v>5.2236700000000003</v>
+      </c>
+      <c r="AF17" s="21">
+        <f>(AE17-$D17)</f>
+        <v>3.5604700000000999</v>
+      </c>
+      <c r="AG17" s="22">
+        <v>0.19924500000000001</v>
+      </c>
+      <c r="AL17" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="AM17" s="20">
+        <v>5.2236700000000003</v>
+      </c>
+      <c r="AN17" s="21">
+        <f>(AM17-$D17)</f>
+        <v>3.5604700000000999</v>
+      </c>
+      <c r="AO17" s="22">
+        <v>0.22884399999999999</v>
+      </c>
+      <c r="AT17" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="AU17" s="20">
+        <v>11.9445</v>
+      </c>
+      <c r="AV17" s="21">
+        <f>(AU17-$D17)</f>
+        <v>10.281300000000099</v>
+      </c>
+      <c r="AW17" s="22">
+        <v>0.14855199999999999</v>
+      </c>
+      <c r="BB17" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="BC17" s="20">
+        <v>8.1311800000000005</v>
+      </c>
+      <c r="BD17" s="21">
+        <f>(BC17-$D17)</f>
+        <v>6.4679800000001002</v>
+      </c>
+      <c r="BE17" s="22">
+        <v>0.14971499999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:57" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>24</v>
       </c>
@@ -2747,8 +3791,60 @@
       <c r="Y18" s="22">
         <v>2.9310799999999999E-4</v>
       </c>
-    </row>
-    <row r="19" spans="1:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD18" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE18" s="20">
+        <v>4.9414999999999996</v>
+      </c>
+      <c r="AF18" s="21">
+        <f>(AE18-$D18)</f>
+        <v>2.0883700000000394</v>
+      </c>
+      <c r="AG18" s="22">
+        <v>0.20553399999999999</v>
+      </c>
+      <c r="AL18" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="AM18" s="20">
+        <v>4.9414999999999996</v>
+      </c>
+      <c r="AN18" s="21">
+        <f>(AM18-$D18)</f>
+        <v>2.0883700000000394</v>
+      </c>
+      <c r="AO18" s="22">
+        <v>0.183588</v>
+      </c>
+      <c r="AT18" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="AU18" s="20">
+        <v>8.8057499999999997</v>
+      </c>
+      <c r="AV18" s="21">
+        <f>(AU18-$D18)</f>
+        <v>5.9526200000000395</v>
+      </c>
+      <c r="AW18" s="22">
+        <v>0.149342</v>
+      </c>
+      <c r="BB18" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="BC18" s="20">
+        <v>11.2965</v>
+      </c>
+      <c r="BD18" s="21">
+        <f>(BC18-$D18)</f>
+        <v>8.4433700000000407</v>
+      </c>
+      <c r="BE18" s="22">
+        <v>0.14816499999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:57" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>25</v>
       </c>
@@ -2807,8 +3903,60 @@
       <c r="Y19" s="22">
         <v>2.2781400000000001E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:25" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD19" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE19" s="20">
+        <v>72.374399999999994</v>
+      </c>
+      <c r="AF19" s="21">
+        <f>(AE19-$D19)</f>
+        <v>29.628620000000893</v>
+      </c>
+      <c r="AG19" s="22">
+        <v>1.35839</v>
+      </c>
+      <c r="AL19" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="AM19" s="20">
+        <v>42.745800000000003</v>
+      </c>
+      <c r="AN19" s="21">
+        <f>(AM19-$D19)</f>
+        <v>2.000000090163212E-5</v>
+      </c>
+      <c r="AO19" s="22">
+        <v>0.76120500000000002</v>
+      </c>
+      <c r="AT19" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="AU19" s="20">
+        <v>42.745800000000003</v>
+      </c>
+      <c r="AV19" s="21">
+        <f>(AU19-$D19)</f>
+        <v>2.000000090163212E-5</v>
+      </c>
+      <c r="AW19" s="22">
+        <v>0.59130300000000002</v>
+      </c>
+      <c r="BB19" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="BC19" s="20">
+        <v>78.565399999999997</v>
+      </c>
+      <c r="BD19" s="21">
+        <f>(BC19-$D19)</f>
+        <v>35.819620000000896</v>
+      </c>
+      <c r="BE19" s="22">
+        <v>0.538628</v>
+      </c>
+    </row>
+    <row r="20" spans="1:57" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>26</v>
       </c>
@@ -2867,8 +4015,60 @@
       <c r="Y20" s="22">
         <v>2.5173299999999999E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:25" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD20" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE20" s="20">
+        <v>59.486800000000002</v>
+      </c>
+      <c r="AF20" s="21">
+        <f>(AE20-$D20)</f>
+        <v>11.379190000000399</v>
+      </c>
+      <c r="AG20" s="22">
+        <v>1.3980999999999999</v>
+      </c>
+      <c r="AL20" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM20" s="20">
+        <v>84.571899999999999</v>
+      </c>
+      <c r="AN20" s="21">
+        <f>(AM20-$D20)</f>
+        <v>36.464290000000396</v>
+      </c>
+      <c r="AO20" s="22">
+        <v>0.73078399999999999</v>
+      </c>
+      <c r="AT20" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="AU20" s="20">
+        <v>84.408699999999996</v>
+      </c>
+      <c r="AV20" s="21">
+        <f>(AU20-$D20)</f>
+        <v>36.301090000000393</v>
+      </c>
+      <c r="AW20" s="22">
+        <v>0.58935800000000005</v>
+      </c>
+      <c r="BB20" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="BC20" s="20">
+        <v>88.621300000000005</v>
+      </c>
+      <c r="BD20" s="21">
+        <f>(BC20-$D20)</f>
+        <v>40.513690000000402</v>
+      </c>
+      <c r="BE20" s="22">
+        <v>0.53232500000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:57" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>27</v>
       </c>
@@ -2927,8 +4127,60 @@
       <c r="Y21" s="22">
         <v>2.5834400000000002E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:25" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD21" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE21" s="20">
+        <v>53.575899999999997</v>
+      </c>
+      <c r="AF21" s="21">
+        <f>(AE21-$D21)</f>
+        <v>10.379810000000298</v>
+      </c>
+      <c r="AG21" s="22">
+        <v>1.5136799999999999</v>
+      </c>
+      <c r="AL21" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="AM21" s="20">
+        <v>66.146799999999999</v>
+      </c>
+      <c r="AN21" s="21">
+        <f>(AM21-$D21)</f>
+        <v>22.950710000000299</v>
+      </c>
+      <c r="AO21" s="22">
+        <v>0.67774800000000002</v>
+      </c>
+      <c r="AT21" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="AU21" s="20">
+        <v>56.945300000000003</v>
+      </c>
+      <c r="AV21" s="21">
+        <f>(AU21-$D21)</f>
+        <v>13.749210000000303</v>
+      </c>
+      <c r="AW21" s="22">
+        <v>0.57465500000000003</v>
+      </c>
+      <c r="BB21" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="BC21" s="20">
+        <v>43.196100000000001</v>
+      </c>
+      <c r="BD21" s="21">
+        <f>(BC21-$D21)</f>
+        <v>1.0000000301602086E-5</v>
+      </c>
+      <c r="BE21" s="22">
+        <v>0.53485000000000005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:57" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
         <v>28</v>
       </c>
@@ -2987,8 +4239,60 @@
       <c r="Y22" s="22">
         <v>2.4315500000000002E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:25" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD22" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE22" s="20">
+        <v>59.2819</v>
+      </c>
+      <c r="AF22" s="21">
+        <f>(AE22-$D22)</f>
+        <v>12.869450000000597</v>
+      </c>
+      <c r="AG22" s="22">
+        <v>1.4336100000000001</v>
+      </c>
+      <c r="AL22" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="AM22" s="20">
+        <v>53.8508</v>
+      </c>
+      <c r="AN22" s="21">
+        <f>(AM22-$D22)</f>
+        <v>7.4383500000005967</v>
+      </c>
+      <c r="AO22" s="22">
+        <v>0.71797299999999997</v>
+      </c>
+      <c r="AT22" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="AU22" s="20">
+        <v>63.693399999999997</v>
+      </c>
+      <c r="AV22" s="21">
+        <f>(AU22-$D22)</f>
+        <v>17.280950000000594</v>
+      </c>
+      <c r="AW22" s="22">
+        <v>0.62547799999999998</v>
+      </c>
+      <c r="BB22" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="BC22" s="20">
+        <v>71.637200000000007</v>
+      </c>
+      <c r="BD22" s="21">
+        <f>(BC22-$D22)</f>
+        <v>25.224750000000604</v>
+      </c>
+      <c r="BE22" s="22">
+        <v>0.53361599999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:57" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>29</v>
       </c>
@@ -3047,8 +4351,60 @@
       <c r="Y23" s="22">
         <v>2.0147099999999999E-3</v>
       </c>
-    </row>
-    <row r="24" spans="1:25" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD23" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE23" s="20">
+        <v>47.7151</v>
+      </c>
+      <c r="AF23" s="21">
+        <f>(AE23-$D23)</f>
+        <v>-9.9999995981647771E-6</v>
+      </c>
+      <c r="AG23" s="22">
+        <v>1.3048299999999999</v>
+      </c>
+      <c r="AL23" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM23" s="20">
+        <v>88.512200000000007</v>
+      </c>
+      <c r="AN23" s="21">
+        <f>(AM23-$D23)</f>
+        <v>40.797090000000409</v>
+      </c>
+      <c r="AO23" s="22">
+        <v>0.73074300000000003</v>
+      </c>
+      <c r="AT23" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AU23" s="20">
+        <v>58.883400000000002</v>
+      </c>
+      <c r="AV23" s="21">
+        <f>(AU23-$D23)</f>
+        <v>11.168290000000404</v>
+      </c>
+      <c r="AW23" s="22">
+        <v>0.59067000000000003</v>
+      </c>
+      <c r="BB23" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="BC23" s="20">
+        <v>74.425399999999996</v>
+      </c>
+      <c r="BD23" s="21">
+        <f>(BC23-$D23)</f>
+        <v>26.710290000000398</v>
+      </c>
+      <c r="BE23" s="22">
+        <v>0.53663799999999995</v>
+      </c>
+    </row>
+    <row r="24" spans="1:57" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
         <v>30</v>
       </c>
@@ -3107,8 +4463,60 @@
       <c r="Y24" s="22">
         <v>2.3437699999999998E-3</v>
       </c>
-    </row>
-    <row r="25" spans="1:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD24" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE24" s="20">
+        <v>30.020199999999999</v>
+      </c>
+      <c r="AF24" s="21">
+        <f>(AE24-$D24)</f>
+        <v>16.188180000000099</v>
+      </c>
+      <c r="AG24" s="22">
+        <v>1.2236800000000001</v>
+      </c>
+      <c r="AL24" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="AM24" s="20">
+        <v>29.296399999999998</v>
+      </c>
+      <c r="AN24" s="21">
+        <f>(AM24-$D24)</f>
+        <v>15.464380000000098</v>
+      </c>
+      <c r="AO24" s="22">
+        <v>0.42435899999999999</v>
+      </c>
+      <c r="AT24" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="AU24" s="20">
+        <v>30.188700000000001</v>
+      </c>
+      <c r="AV24" s="21">
+        <f>(AU24-$D24)</f>
+        <v>16.3566800000001</v>
+      </c>
+      <c r="AW24" s="22">
+        <v>0.34496199999999999</v>
+      </c>
+      <c r="BB24" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="BC24" s="20">
+        <v>26.769300000000001</v>
+      </c>
+      <c r="BD24" s="21">
+        <f>(BC24-$D24)</f>
+        <v>12.937280000000101</v>
+      </c>
+      <c r="BE24" s="22">
+        <v>0.31827899999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:57" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>31</v>
       </c>
@@ -3161,8 +4569,60 @@
       <c r="Y25" s="22">
         <v>2.0449600000000002E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD25" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE25" s="20">
+        <v>23.1114</v>
+      </c>
+      <c r="AF25" s="21">
+        <f>(AE25-$D25)</f>
+        <v>9.4470599999997003</v>
+      </c>
+      <c r="AG25" s="22">
+        <v>0.82628100000000004</v>
+      </c>
+      <c r="AL25" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM25" s="20">
+        <v>32.048099999999998</v>
+      </c>
+      <c r="AN25" s="21">
+        <f>(AM25-$D25)</f>
+        <v>18.383759999999697</v>
+      </c>
+      <c r="AO25" s="22">
+        <v>0.39522000000000002</v>
+      </c>
+      <c r="AT25" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="AU25" s="20">
+        <v>31.646999999999998</v>
+      </c>
+      <c r="AV25" s="21">
+        <f>(AU25-$D25)</f>
+        <v>17.982659999999697</v>
+      </c>
+      <c r="AW25" s="22">
+        <v>0.330154</v>
+      </c>
+      <c r="BB25" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="BC25" s="20">
+        <v>37.0349</v>
+      </c>
+      <c r="BD25" s="21">
+        <f>(BC25-$D25)</f>
+        <v>23.370559999999699</v>
+      </c>
+      <c r="BE25" s="22">
+        <v>0.31646999999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:57" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
         <v>32</v>
       </c>
@@ -3215,8 +4675,60 @@
       <c r="Y26" s="22">
         <v>2.2048900000000001E-3</v>
       </c>
-    </row>
-    <row r="27" spans="1:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD26" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE26" s="20">
+        <v>20.6145</v>
+      </c>
+      <c r="AF26" s="21">
+        <f>(AE26-$D26)</f>
+        <v>5.2691200000001999</v>
+      </c>
+      <c r="AG26" s="22">
+        <v>0.750946</v>
+      </c>
+      <c r="AL26" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM26" s="20">
+        <v>37.847700000000003</v>
+      </c>
+      <c r="AN26" s="21">
+        <f>(AM26-$D26)</f>
+        <v>22.502320000000203</v>
+      </c>
+      <c r="AO26" s="22">
+        <v>0.37772699999999998</v>
+      </c>
+      <c r="AT26" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU26" s="20">
+        <v>16.451699999999999</v>
+      </c>
+      <c r="AV26" s="21">
+        <f>(AU26-$D26)</f>
+        <v>1.1063200000001991</v>
+      </c>
+      <c r="AW26" s="22">
+        <v>0.33670499999999998</v>
+      </c>
+      <c r="BB26" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="BC26" s="20">
+        <v>23.909500000000001</v>
+      </c>
+      <c r="BD26" s="21">
+        <f>(BC26-$D26)</f>
+        <v>8.5641200000002016</v>
+      </c>
+      <c r="BE26" s="22">
+        <v>0.31766800000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:57" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
         <v>33</v>
       </c>
@@ -3269,8 +4781,60 @@
       <c r="Y27" s="22">
         <v>2.3582799999999999E-3</v>
       </c>
-    </row>
-    <row r="28" spans="1:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD27" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE27" s="20">
+        <v>22.187999999999999</v>
+      </c>
+      <c r="AF27" s="21">
+        <f>(AE27-$D27)</f>
+        <v>13.547360000000609</v>
+      </c>
+      <c r="AG27" s="22">
+        <v>0.85583299999999995</v>
+      </c>
+      <c r="AL27" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM27" s="20">
+        <v>31.458200000000001</v>
+      </c>
+      <c r="AN27" s="21">
+        <f>(AM27-$D27)</f>
+        <v>22.817560000000611</v>
+      </c>
+      <c r="AO27" s="22">
+        <v>0.39744000000000002</v>
+      </c>
+      <c r="AT27" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="AU27" s="20">
+        <v>32.114899999999999</v>
+      </c>
+      <c r="AV27" s="21">
+        <f>(AU27-$D27)</f>
+        <v>23.474260000000609</v>
+      </c>
+      <c r="AW27" s="22">
+        <v>0.33551799999999998</v>
+      </c>
+      <c r="BB27" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="BC27" s="20">
+        <v>36.4542</v>
+      </c>
+      <c r="BD27" s="21">
+        <f>(BC27-$D27)</f>
+        <v>27.81356000000061</v>
+      </c>
+      <c r="BE27" s="22">
+        <v>0.31965900000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:57" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>34</v>
       </c>
@@ -3323,8 +4887,60 @@
       <c r="Y28" s="22">
         <v>2.1693099999999998E-3</v>
       </c>
-    </row>
-    <row r="29" spans="1:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD28" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE28" s="20">
+        <v>21.111000000000001</v>
+      </c>
+      <c r="AF28" s="21">
+        <f>(AE28-$D28)</f>
+        <v>3.9104900000001024</v>
+      </c>
+      <c r="AG28" s="22">
+        <v>0.82885900000000001</v>
+      </c>
+      <c r="AL28" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="AM28" s="20">
+        <v>27.530200000000001</v>
+      </c>
+      <c r="AN28" s="21">
+        <f>(AM28-$D28)</f>
+        <v>10.329690000000102</v>
+      </c>
+      <c r="AO28" s="22">
+        <v>0.38570300000000002</v>
+      </c>
+      <c r="AT28" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="AU28" s="20">
+        <v>22.794599999999999</v>
+      </c>
+      <c r="AV28" s="21">
+        <f>(AU28-$D28)</f>
+        <v>5.5940900000001008</v>
+      </c>
+      <c r="AW28" s="22">
+        <v>0.34825099999999998</v>
+      </c>
+      <c r="BB28" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="BC28" s="20">
+        <v>22.216799999999999</v>
+      </c>
+      <c r="BD28" s="21">
+        <f>(BC28-$D28)</f>
+        <v>5.0162900000001009</v>
+      </c>
+      <c r="BE28" s="22">
+        <v>0.31817899999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:57" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>35</v>
       </c>
@@ -3377,8 +4993,60 @@
       <c r="Y29" s="22">
         <v>2.1916999999999999E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:25" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD29" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE29" s="20">
+        <v>298.858</v>
+      </c>
+      <c r="AF29" s="21">
+        <f>(AE29-$D29)</f>
+        <v>130.12840999999901</v>
+      </c>
+      <c r="AG29" s="22">
+        <v>7.8428699999999996</v>
+      </c>
+      <c r="AL29" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="AM29" s="20">
+        <v>406.09800000000001</v>
+      </c>
+      <c r="AN29" s="21">
+        <f>(AM29-$D29)</f>
+        <v>237.36840999999902</v>
+      </c>
+      <c r="AO29" s="22">
+        <v>1.89777</v>
+      </c>
+      <c r="AT29" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="AU29" s="20">
+        <v>203.94</v>
+      </c>
+      <c r="AV29" s="21">
+        <f>(AU29-$D29)</f>
+        <v>35.210409999999001</v>
+      </c>
+      <c r="AW29" s="22">
+        <v>10.0877</v>
+      </c>
+      <c r="BB29" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="BC29" s="20">
+        <v>179.221</v>
+      </c>
+      <c r="BD29" s="21">
+        <f>(BC29-$D29)</f>
+        <v>10.491409999999007</v>
+      </c>
+      <c r="BE29" s="22">
+        <v>1.5713999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:57" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>36</v>
       </c>
@@ -3437,8 +5105,60 @@
       <c r="Y30" s="22">
         <v>1.7515200000000002E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD30" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE30" s="20">
+        <v>270.04899999999998</v>
+      </c>
+      <c r="AF30" s="21">
+        <f>(AE30-$D30)</f>
+        <v>142.95173999999997</v>
+      </c>
+      <c r="AG30" s="22">
+        <v>8.0890000000000004</v>
+      </c>
+      <c r="AL30" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM30" s="20">
+        <v>334.90699999999998</v>
+      </c>
+      <c r="AN30" s="21">
+        <f>(AM30-$D30)</f>
+        <v>207.80973999999998</v>
+      </c>
+      <c r="AO30" s="22">
+        <v>1.91974</v>
+      </c>
+      <c r="AT30" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU30" s="20">
+        <v>150.24799999999999</v>
+      </c>
+      <c r="AV30" s="21">
+        <f>(AU30-$D30)</f>
+        <v>23.150739999999985</v>
+      </c>
+      <c r="AW30" s="22">
+        <v>10.4054</v>
+      </c>
+      <c r="BB30" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="BC30" s="20">
+        <v>182.93700000000001</v>
+      </c>
+      <c r="BD30" s="21">
+        <f>(BC30-$D30)</f>
+        <v>55.839740000000006</v>
+      </c>
+      <c r="BE30" s="22">
+        <v>1.5587500000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:57" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
         <v>37</v>
       </c>
@@ -3491,8 +5211,60 @@
       <c r="Y31" s="22">
         <v>1.76299E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD31" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE31" s="20">
+        <v>266.375</v>
+      </c>
+      <c r="AF31" s="21">
+        <f>(AE31-$D31)</f>
+        <v>159.995810000001</v>
+      </c>
+      <c r="AG31" s="22">
+        <v>7.9219999999999997</v>
+      </c>
+      <c r="AL31" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM31" s="20">
+        <v>372.85300000000001</v>
+      </c>
+      <c r="AN31" s="21">
+        <f>(AM31-$D31)</f>
+        <v>266.47381000000098</v>
+      </c>
+      <c r="AO31" s="22">
+        <v>1.95974</v>
+      </c>
+      <c r="AT31" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="AU31" s="20">
+        <v>164.85300000000001</v>
+      </c>
+      <c r="AV31" s="21">
+        <f>(AU31-$D31)</f>
+        <v>58.473810000001009</v>
+      </c>
+      <c r="AW31" s="22">
+        <v>8.7870699999999999</v>
+      </c>
+      <c r="BB31" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="BC31" s="20">
+        <v>231.56399999999999</v>
+      </c>
+      <c r="BD31" s="21">
+        <f>(BC31-$D31)</f>
+        <v>125.18481000000099</v>
+      </c>
+      <c r="BE31" s="22">
+        <v>1.5217000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:57" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
         <v>38</v>
       </c>
@@ -3545,8 +5317,60 @@
       <c r="Y32" s="22">
         <v>2.5472000000000002E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD32" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE32" s="20">
+        <v>224.208</v>
+      </c>
+      <c r="AF32" s="21">
+        <f>(AE32-$D32)</f>
+        <v>86.754840000000996</v>
+      </c>
+      <c r="AG32" s="22">
+        <v>7.9828799999999998</v>
+      </c>
+      <c r="AL32" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM32" s="20">
+        <v>345.31400000000002</v>
+      </c>
+      <c r="AN32" s="21">
+        <f>(AM32-$D32)</f>
+        <v>207.86084000000102</v>
+      </c>
+      <c r="AO32" s="22">
+        <v>1.9214800000000001</v>
+      </c>
+      <c r="AT32" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="AU32" s="20">
+        <v>153.011</v>
+      </c>
+      <c r="AV32" s="21">
+        <f>(AU32-$D32)</f>
+        <v>15.557840000000994</v>
+      </c>
+      <c r="AW32" s="22">
+        <v>10.1335</v>
+      </c>
+      <c r="BB32" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="BC32" s="20">
+        <v>211.239</v>
+      </c>
+      <c r="BD32" s="21">
+        <f>(BC32-$D32)</f>
+        <v>73.785840000001002</v>
+      </c>
+      <c r="BE32" s="22">
+        <v>1.51004</v>
+      </c>
+    </row>
+    <row r="33" spans="1:57" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
         <v>39</v>
       </c>
@@ -3599,8 +5423,60 @@
       <c r="Y33" s="22">
         <v>1.8075600000000001E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD33" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE33" s="20">
+        <v>245.881</v>
+      </c>
+      <c r="AF33" s="21">
+        <f>(AE33-$D33)</f>
+        <v>118.401259999999</v>
+      </c>
+      <c r="AG33" s="22">
+        <v>7.9211200000000002</v>
+      </c>
+      <c r="AL33" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="AM33" s="20">
+        <v>321.93900000000002</v>
+      </c>
+      <c r="AN33" s="21">
+        <f>(AM33-$D33)</f>
+        <v>194.45925999999901</v>
+      </c>
+      <c r="AO33" s="22">
+        <v>1.93292</v>
+      </c>
+      <c r="AT33" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="AU33" s="20">
+        <v>151.43899999999999</v>
+      </c>
+      <c r="AV33" s="21">
+        <f>(AU33-$D33)</f>
+        <v>23.959259999998991</v>
+      </c>
+      <c r="AW33" s="22">
+        <v>9.0530200000000001</v>
+      </c>
+      <c r="BB33" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="BC33" s="20">
+        <v>221.36799999999999</v>
+      </c>
+      <c r="BD33" s="21">
+        <f>(BC33-$D33)</f>
+        <v>93.888259999998994</v>
+      </c>
+      <c r="BE33" s="22">
+        <v>1.64838</v>
+      </c>
+    </row>
+    <row r="34" spans="1:57" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
         <v>40</v>
       </c>
@@ -3653,8 +5529,60 @@
       <c r="Y34" s="22">
         <v>5.3389500000000003E-3</v>
       </c>
-    </row>
-    <row r="35" spans="1:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD34" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE34" s="20">
+        <v>38.359099999999998</v>
+      </c>
+      <c r="AF34" s="21">
+        <f>(AE34-$D34)</f>
+        <v>26.613960000000098</v>
+      </c>
+      <c r="AG34" s="22">
+        <v>1.19129</v>
+      </c>
+      <c r="AL34" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM34" s="20">
+        <v>35.745600000000003</v>
+      </c>
+      <c r="AN34" s="21">
+        <f>(AM34-$D34)</f>
+        <v>24.000460000000103</v>
+      </c>
+      <c r="AO34" s="22">
+        <v>0.51712599999999997</v>
+      </c>
+      <c r="AT34" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AU34" s="20">
+        <v>42.117199999999997</v>
+      </c>
+      <c r="AV34" s="21">
+        <f>(AU34-$D34)</f>
+        <v>30.372060000000097</v>
+      </c>
+      <c r="AW34" s="22">
+        <v>0.43601400000000001</v>
+      </c>
+      <c r="BB34" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="BC34" s="20">
+        <v>43.256999999999998</v>
+      </c>
+      <c r="BD34" s="21">
+        <f>(BC34-$D34)</f>
+        <v>31.511860000000098</v>
+      </c>
+      <c r="BE34" s="22">
+        <v>0.39006400000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:57" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
         <v>41</v>
       </c>
@@ -3707,8 +5635,60 @@
       <c r="Y35" s="22">
         <v>4.1190200000000001E-3</v>
       </c>
-    </row>
-    <row r="36" spans="1:25" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD35" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE35" s="20">
+        <v>27.086200000000002</v>
+      </c>
+      <c r="AF35" s="21">
+        <f>(AE35-$D35)</f>
+        <v>8.297270000000303</v>
+      </c>
+      <c r="AG35" s="22">
+        <v>1.22506</v>
+      </c>
+      <c r="AL35" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM35" s="20">
+        <v>30.793900000000001</v>
+      </c>
+      <c r="AN35" s="21">
+        <f>(AM35-$D35)</f>
+        <v>12.004970000000302</v>
+      </c>
+      <c r="AO35" s="22">
+        <v>0.49638900000000002</v>
+      </c>
+      <c r="AT35" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="AU35" s="20">
+        <v>41.699399999999997</v>
+      </c>
+      <c r="AV35" s="21">
+        <f>(AU35-$D35)</f>
+        <v>22.910470000000299</v>
+      </c>
+      <c r="AW35" s="22">
+        <v>0.43721199999999999</v>
+      </c>
+      <c r="BB35" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="BC35" s="20">
+        <v>38.170299999999997</v>
+      </c>
+      <c r="BD35" s="21">
+        <f>(BC35-$D35)</f>
+        <v>19.381370000000299</v>
+      </c>
+      <c r="BE35" s="22">
+        <v>0.385828</v>
+      </c>
+    </row>
+    <row r="36" spans="1:57" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
         <v>42</v>
       </c>
@@ -3761,14 +5741,66 @@
         <v>70.190399999999997</v>
       </c>
       <c r="X36" s="21">
-        <f t="shared" ref="X36:X67" si="3">(W36-$D36)</f>
+        <f t="shared" ref="X36:X53" si="3">(W36-$D36)</f>
         <v>51.658800000000198</v>
       </c>
       <c r="Y36" s="22">
         <v>4.3060399999999997E-3</v>
       </c>
-    </row>
-    <row r="37" spans="1:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD36" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE36" s="20">
+        <v>22.4956</v>
+      </c>
+      <c r="AF36" s="21">
+        <f>(AE36-$D36)</f>
+        <v>3.9640000000002011</v>
+      </c>
+      <c r="AG36" s="22">
+        <v>1.2315100000000001</v>
+      </c>
+      <c r="AL36" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM36" s="20">
+        <v>29.9572</v>
+      </c>
+      <c r="AN36" s="21">
+        <f>(AM36-$D36)</f>
+        <v>11.425600000000202</v>
+      </c>
+      <c r="AO36" s="22">
+        <v>0.515513</v>
+      </c>
+      <c r="AT36" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="AU36" s="20">
+        <v>25.5398</v>
+      </c>
+      <c r="AV36" s="21">
+        <f>(AU36-$D36)</f>
+        <v>7.0082000000002012</v>
+      </c>
+      <c r="AW36" s="22">
+        <v>0.44154500000000002</v>
+      </c>
+      <c r="BB36" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="BC36" s="20">
+        <v>42.520099999999999</v>
+      </c>
+      <c r="BD36" s="21">
+        <f>(BC36-$D36)</f>
+        <v>23.988500000000201</v>
+      </c>
+      <c r="BE36" s="22">
+        <v>0.38494600000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:57" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
         <v>43</v>
       </c>
@@ -3820,8 +5852,60 @@
       <c r="Y37" s="22">
         <v>4.0950800000000001E-3</v>
       </c>
-    </row>
-    <row r="38" spans="1:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD37" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE37" s="20">
+        <v>35.639400000000002</v>
+      </c>
+      <c r="AF37" s="21">
+        <f>(AE37-$D37)</f>
+        <v>16.151069999999901</v>
+      </c>
+      <c r="AG37" s="22">
+        <v>1.2012700000000001</v>
+      </c>
+      <c r="AL37" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="AM37" s="20">
+        <v>37.859200000000001</v>
+      </c>
+      <c r="AN37" s="21">
+        <f>(AM37-$D37)</f>
+        <v>18.370869999999901</v>
+      </c>
+      <c r="AO37" s="22">
+        <v>0.52687300000000004</v>
+      </c>
+      <c r="AT37" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="AU37" s="20">
+        <v>28.215299999999999</v>
+      </c>
+      <c r="AV37" s="21">
+        <f>(AU37-$D37)</f>
+        <v>8.7269699999998984</v>
+      </c>
+      <c r="AW37" s="22">
+        <v>0.47076499999999999</v>
+      </c>
+      <c r="BB37" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="BC37" s="20">
+        <v>29.6037</v>
+      </c>
+      <c r="BD37" s="21">
+        <f>(BC37-$D37)</f>
+        <v>10.115369999999899</v>
+      </c>
+      <c r="BE37" s="22">
+        <v>0.38878299999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:57" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
         <v>44</v>
       </c>
@@ -3873,8 +5957,60 @@
       <c r="Y38" s="22">
         <v>4.5113799999999997E-3</v>
       </c>
-    </row>
-    <row r="39" spans="1:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD38" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE38" s="20">
+        <v>31.1067</v>
+      </c>
+      <c r="AF38" s="21">
+        <f>(AE38-$D38)</f>
+        <v>12.994280000000199</v>
+      </c>
+      <c r="AG38" s="22">
+        <v>1.2196400000000001</v>
+      </c>
+      <c r="AL38" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM38" s="20">
+        <v>40.652099999999997</v>
+      </c>
+      <c r="AN38" s="21">
+        <f>(AM38-$D38)</f>
+        <v>22.539680000000196</v>
+      </c>
+      <c r="AO38" s="22">
+        <v>0.51843799999999995</v>
+      </c>
+      <c r="AT38" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU38" s="20">
+        <v>29.9754</v>
+      </c>
+      <c r="AV38" s="21">
+        <f>(AU38-$D38)</f>
+        <v>11.862980000000199</v>
+      </c>
+      <c r="AW38" s="22">
+        <v>0.43558799999999998</v>
+      </c>
+      <c r="BB38" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="BC38" s="20">
+        <v>25.328299999999999</v>
+      </c>
+      <c r="BD38" s="21">
+        <f>(BC38-$D38)</f>
+        <v>7.2158800000001975</v>
+      </c>
+      <c r="BE38" s="22">
+        <v>0.38973099999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:57" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
         <v>45</v>
       </c>
@@ -3926,8 +6062,60 @@
       <c r="Y39" s="22">
         <v>4.2894399999999999E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD39" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE39" s="20">
+        <v>354.779</v>
+      </c>
+      <c r="AF39" s="21">
+        <f>(AE39-$D39)</f>
+        <v>199.34422999999799</v>
+      </c>
+      <c r="AG39" s="22">
+        <v>14.5411</v>
+      </c>
+      <c r="AL39" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="AM39" s="20">
+        <v>405.815</v>
+      </c>
+      <c r="AN39" s="21">
+        <f>(AM39-$D39)</f>
+        <v>250.38022999999799</v>
+      </c>
+      <c r="AO39" s="22">
+        <v>2.9821900000000001</v>
+      </c>
+      <c r="AT39" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU39" s="20">
+        <v>210.54599999999999</v>
+      </c>
+      <c r="AV39" s="21">
+        <f>(AU39-$D39)</f>
+        <v>55.111229999997988</v>
+      </c>
+      <c r="AW39" s="22">
+        <v>23.977499999999999</v>
+      </c>
+      <c r="BB39" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="BC39" s="20">
+        <v>198.78100000000001</v>
+      </c>
+      <c r="BD39" s="21">
+        <f>(BC39-$D39)</f>
+        <v>43.346229999998002</v>
+      </c>
+      <c r="BE39" s="22">
+        <v>2.39886</v>
+      </c>
+    </row>
+    <row r="40" spans="1:57" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
         <v>46</v>
       </c>
@@ -3979,8 +6167,60 @@
       <c r="Y40" s="22">
         <v>4.0776800000000002E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD40" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE40" s="20">
+        <v>484.375</v>
+      </c>
+      <c r="AF40" s="21">
+        <f>(AE40-$D40)</f>
+        <v>285.48038000000099</v>
+      </c>
+      <c r="AG40" s="22">
+        <v>14.8467</v>
+      </c>
+      <c r="AL40" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AM40" s="20">
+        <v>468.75799999999998</v>
+      </c>
+      <c r="AN40" s="21">
+        <f>(AM40-$D40)</f>
+        <v>269.86338000000097</v>
+      </c>
+      <c r="AO40" s="22">
+        <v>2.6215000000000002</v>
+      </c>
+      <c r="AT40" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="AU40" s="20">
+        <v>273.00799999999998</v>
+      </c>
+      <c r="AV40" s="21">
+        <f>(AU40-$D40)</f>
+        <v>74.113380000000973</v>
+      </c>
+      <c r="AW40" s="22">
+        <v>27.215499999999999</v>
+      </c>
+      <c r="BB40" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="BC40" s="20">
+        <v>307.50099999999998</v>
+      </c>
+      <c r="BD40" s="21">
+        <f>(BC40-$D40)</f>
+        <v>108.60638000000097</v>
+      </c>
+      <c r="BE40" s="22">
+        <v>2.1698400000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:57" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="18" t="s">
         <v>47</v>
       </c>
@@ -4032,8 +6272,60 @@
       <c r="Y41" s="22">
         <v>4.4387799999999998E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:25" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD41" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE41" s="20">
+        <v>416.108</v>
+      </c>
+      <c r="AF41" s="21">
+        <f>(AE41-$D41)</f>
+        <v>228.14097000000001</v>
+      </c>
+      <c r="AG41" s="22">
+        <v>14.4475</v>
+      </c>
+      <c r="AL41" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="AM41" s="20">
+        <v>517.21799999999996</v>
+      </c>
+      <c r="AN41" s="21">
+        <f>(AM41-$D41)</f>
+        <v>329.25096999999994</v>
+      </c>
+      <c r="AO41" s="22">
+        <v>2.60684</v>
+      </c>
+      <c r="AT41" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="AU41" s="20">
+        <v>271.262</v>
+      </c>
+      <c r="AV41" s="21">
+        <f>(AU41-$D41)</f>
+        <v>83.294970000000006</v>
+      </c>
+      <c r="AW41" s="22">
+        <v>29.023299999999999</v>
+      </c>
+      <c r="BB41" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="BC41" s="20">
+        <v>310.14600000000002</v>
+      </c>
+      <c r="BD41" s="21">
+        <f>(BC41-$D41)</f>
+        <v>122.17897000000002</v>
+      </c>
+      <c r="BE41" s="22">
+        <v>2.3606500000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:57" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
         <v>48</v>
       </c>
@@ -4092,8 +6384,60 @@
       <c r="Y42" s="22">
         <v>4.3107399999999997E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD42" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE42" s="20">
+        <v>359.15</v>
+      </c>
+      <c r="AF42" s="21">
+        <f>(AE42-$D42)</f>
+        <v>190.55979999999897</v>
+      </c>
+      <c r="AG42" s="22">
+        <v>14.3384</v>
+      </c>
+      <c r="AL42" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="AM42" s="20">
+        <v>452.29399999999998</v>
+      </c>
+      <c r="AN42" s="21">
+        <f>(AM42-$D42)</f>
+        <v>283.70379999999898</v>
+      </c>
+      <c r="AO42" s="22">
+        <v>2.5411700000000002</v>
+      </c>
+      <c r="AT42" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="AU42" s="20">
+        <v>226.107</v>
+      </c>
+      <c r="AV42" s="21">
+        <f>(AU42-$D42)</f>
+        <v>57.516799999998995</v>
+      </c>
+      <c r="AW42" s="22">
+        <v>26.388300000000001</v>
+      </c>
+      <c r="BB42" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="BC42" s="20">
+        <v>220.988</v>
+      </c>
+      <c r="BD42" s="21">
+        <f>(BC42-$D42)</f>
+        <v>52.397799999998995</v>
+      </c>
+      <c r="BE42" s="22">
+        <v>2.2989600000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:57" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
         <v>49</v>
       </c>
@@ -4146,8 +6490,60 @@
       <c r="Y43" s="22">
         <v>3.8445800000000002E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD43" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE43" s="20">
+        <v>465.48599999999999</v>
+      </c>
+      <c r="AF43" s="21">
+        <f>(AE43-$D43)</f>
+        <v>287.29225999999699</v>
+      </c>
+      <c r="AG43" s="22">
+        <v>14.3901</v>
+      </c>
+      <c r="AL43" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="AM43" s="20">
+        <v>549.94399999999996</v>
+      </c>
+      <c r="AN43" s="21">
+        <f>(AM43-$D43)</f>
+        <v>371.75025999999696</v>
+      </c>
+      <c r="AO43" s="22">
+        <v>2.7884500000000001</v>
+      </c>
+      <c r="AT43" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="AU43" s="20">
+        <v>319.88299999999998</v>
+      </c>
+      <c r="AV43" s="21">
+        <f>(AU43-$D43)</f>
+        <v>141.68925999999698</v>
+      </c>
+      <c r="AW43" s="22">
+        <v>27.511700000000001</v>
+      </c>
+      <c r="BB43" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="BC43" s="20">
+        <v>266.62400000000002</v>
+      </c>
+      <c r="BD43" s="21">
+        <f>(BC43-$D43)</f>
+        <v>88.43025999999702</v>
+      </c>
+      <c r="BE43" s="22">
+        <v>2.20662</v>
+      </c>
+    </row>
+    <row r="44" spans="1:57" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
         <v>50</v>
       </c>
@@ -4206,8 +6602,60 @@
       <c r="Y44" s="22">
         <v>6.6451599999999998E-3</v>
       </c>
-    </row>
-    <row r="45" spans="1:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD44" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE44" s="20">
+        <v>49.547499999999999</v>
+      </c>
+      <c r="AF44" s="21">
+        <f>(AE44-$D44)</f>
+        <v>26.2014199999997</v>
+      </c>
+      <c r="AG44" s="22">
+        <v>2.1995100000000001</v>
+      </c>
+      <c r="AL44" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM44" s="20">
+        <v>65.522400000000005</v>
+      </c>
+      <c r="AN44" s="21">
+        <f>(AM44-$D44)</f>
+        <v>42.176319999999706</v>
+      </c>
+      <c r="AO44" s="22">
+        <v>0.69735800000000003</v>
+      </c>
+      <c r="AT44" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="AU44" s="20">
+        <v>31.984400000000001</v>
+      </c>
+      <c r="AV44" s="21">
+        <f>(AU44-$D44)</f>
+        <v>8.6383199999997018</v>
+      </c>
+      <c r="AW44" s="22">
+        <v>0.69613400000000003</v>
+      </c>
+      <c r="BB44" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="BC44" s="20">
+        <v>57.029899999999998</v>
+      </c>
+      <c r="BD44" s="21">
+        <f>(BC44-$D44)</f>
+        <v>33.683819999999699</v>
+      </c>
+      <c r="BE44" s="22">
+        <v>0.53146599999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:57" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
         <v>51</v>
       </c>
@@ -4260,8 +6708,60 @@
       <c r="Y45" s="22">
         <v>8.1582600000000005E-3</v>
       </c>
-    </row>
-    <row r="46" spans="1:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD45" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE45" s="20">
+        <v>37.251899999999999</v>
+      </c>
+      <c r="AF45" s="21">
+        <f>(AE45-$D45)</f>
+        <v>10.4624000000004</v>
+      </c>
+      <c r="AG45" s="22">
+        <v>2.2263899999999999</v>
+      </c>
+      <c r="AL45" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="AM45" s="20">
+        <v>68.553299999999993</v>
+      </c>
+      <c r="AN45" s="21">
+        <f>(AM45-$D45)</f>
+        <v>41.763800000000394</v>
+      </c>
+      <c r="AO45" s="22">
+        <v>0.724217</v>
+      </c>
+      <c r="AT45" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU45" s="20">
+        <v>46.875500000000002</v>
+      </c>
+      <c r="AV45" s="21">
+        <f>(AU45-$D45)</f>
+        <v>20.086000000000404</v>
+      </c>
+      <c r="AW45" s="22">
+        <v>0.79327800000000004</v>
+      </c>
+      <c r="BB45" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="BC45" s="20">
+        <v>54.901499999999999</v>
+      </c>
+      <c r="BD45" s="21">
+        <f>(BC45-$D45)</f>
+        <v>28.1120000000004</v>
+      </c>
+      <c r="BE45" s="22">
+        <v>0.55542599999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:57" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
         <v>52</v>
       </c>
@@ -4314,8 +6814,60 @@
       <c r="Y46" s="22">
         <v>9.6588200000000003E-3</v>
       </c>
-    </row>
-    <row r="47" spans="1:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD46" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE46" s="20">
+        <v>57.869799999999998</v>
+      </c>
+      <c r="AF46" s="21">
+        <f>(AE46-$D46)</f>
+        <v>31.115330000000398</v>
+      </c>
+      <c r="AG46" s="22">
+        <v>2.1958700000000002</v>
+      </c>
+      <c r="AL46" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM46" s="20">
+        <v>69.658299999999997</v>
+      </c>
+      <c r="AN46" s="21">
+        <f>(AM46-$D46)</f>
+        <v>42.903830000000397</v>
+      </c>
+      <c r="AO46" s="22">
+        <v>0.79368000000000005</v>
+      </c>
+      <c r="AT46" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AU46" s="20">
+        <v>44.9803</v>
+      </c>
+      <c r="AV46" s="21">
+        <f>(AU46-$D46)</f>
+        <v>18.2258300000004</v>
+      </c>
+      <c r="AW46" s="22">
+        <v>0.82750999999999997</v>
+      </c>
+      <c r="BB46" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="BC46" s="20">
+        <v>51.136499999999998</v>
+      </c>
+      <c r="BD46" s="21">
+        <f>(BC46-$D46)</f>
+        <v>24.382030000000398</v>
+      </c>
+      <c r="BE46" s="22">
+        <v>0.53559900000000005</v>
+      </c>
+    </row>
+    <row r="47" spans="1:57" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="18" t="s">
         <v>53</v>
       </c>
@@ -4367,8 +6919,60 @@
       <c r="Y47" s="22">
         <v>8.6810600000000009E-3</v>
       </c>
-    </row>
-    <row r="48" spans="1:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD47" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE47" s="20">
+        <v>57.567399999999999</v>
+      </c>
+      <c r="AF47" s="21">
+        <f>(AE47-$D47)</f>
+        <v>31.631809999999501</v>
+      </c>
+      <c r="AG47" s="22">
+        <v>2.1691199999999999</v>
+      </c>
+      <c r="AL47" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM47" s="20">
+        <v>50.1342</v>
+      </c>
+      <c r="AN47" s="21">
+        <f>(AM47-$D47)</f>
+        <v>24.198609999999501</v>
+      </c>
+      <c r="AO47" s="22">
+        <v>0.74846999999999997</v>
+      </c>
+      <c r="AT47" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AU47" s="20">
+        <v>37.6753</v>
+      </c>
+      <c r="AV47" s="21">
+        <f>(AU47-$D47)</f>
+        <v>11.739709999999501</v>
+      </c>
+      <c r="AW47" s="22">
+        <v>0.79</v>
+      </c>
+      <c r="BB47" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="BC47" s="20">
+        <v>64.764799999999994</v>
+      </c>
+      <c r="BD47" s="21">
+        <f>(BC47-$D47)</f>
+        <v>38.829209999999492</v>
+      </c>
+      <c r="BE47" s="22">
+        <v>0.53243300000000005</v>
+      </c>
+    </row>
+    <row r="48" spans="1:57" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="18" t="s">
         <v>54</v>
       </c>
@@ -4420,8 +7024,60 @@
       <c r="Y48" s="22">
         <v>8.0250500000000006E-3</v>
       </c>
-    </row>
-    <row r="49" spans="1:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD48" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE48" s="20">
+        <v>44.796399999999998</v>
+      </c>
+      <c r="AF48" s="21">
+        <f>(AE48-$D48)</f>
+        <v>17.0233900000006</v>
+      </c>
+      <c r="AG48" s="22">
+        <v>2.3014999999999999</v>
+      </c>
+      <c r="AL48" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM48" s="20">
+        <v>73.726900000000001</v>
+      </c>
+      <c r="AN48" s="21">
+        <f>(AM48-$D48)</f>
+        <v>45.953890000000598</v>
+      </c>
+      <c r="AO48" s="22">
+        <v>0.78282300000000005</v>
+      </c>
+      <c r="AT48" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="AU48" s="20">
+        <v>38.9527</v>
+      </c>
+      <c r="AV48" s="21">
+        <f>(AU48-$D48)</f>
+        <v>11.179690000000601</v>
+      </c>
+      <c r="AW48" s="22">
+        <v>0.86802100000000004</v>
+      </c>
+      <c r="BB48" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="BC48" s="20">
+        <v>43.77</v>
+      </c>
+      <c r="BD48" s="21">
+        <f>(BC48-$D48)</f>
+        <v>15.996990000000604</v>
+      </c>
+      <c r="BE48" s="22">
+        <v>0.53252500000000003</v>
+      </c>
+    </row>
+    <row r="49" spans="1:57" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="18" t="s">
         <v>55</v>
       </c>
@@ -4473,8 +7129,60 @@
       <c r="Y49" s="22">
         <v>7.4335200000000004E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD49" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE49" s="20">
+        <v>642.16</v>
+      </c>
+      <c r="AF49" s="21">
+        <f>(AE49-$D49)</f>
+        <v>414.41069000000198</v>
+      </c>
+      <c r="AG49" s="22">
+        <v>24.888000000000002</v>
+      </c>
+      <c r="AL49" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="AM49" s="20">
+        <v>622.99900000000002</v>
+      </c>
+      <c r="AN49" s="21">
+        <f>(AM49-$D49)</f>
+        <v>395.24969000000203</v>
+      </c>
+      <c r="AO49" s="22">
+        <v>3.5058199999999999</v>
+      </c>
+      <c r="AT49" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU49" s="20">
+        <v>332.74</v>
+      </c>
+      <c r="AV49" s="21">
+        <f>(AU49-$D49)</f>
+        <v>104.99069000000202</v>
+      </c>
+      <c r="AW49" s="22">
+        <v>48.036000000000001</v>
+      </c>
+      <c r="BB49" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="BC49" s="20">
+        <v>490.26799999999997</v>
+      </c>
+      <c r="BD49" s="21">
+        <f>(BC49-$D49)</f>
+        <v>262.51869000000198</v>
+      </c>
+      <c r="BE49" s="22">
+        <v>3.5422199999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:57" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
         <v>56</v>
       </c>
@@ -4526,8 +7234,60 @@
       <c r="Y50" s="22">
         <v>7.3863700000000004E-2</v>
       </c>
-    </row>
-    <row r="51" spans="1:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD50" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE50" s="20">
+        <v>511.976</v>
+      </c>
+      <c r="AF50" s="21">
+        <f>(AE50-$D50)</f>
+        <v>283.37310000000002</v>
+      </c>
+      <c r="AG50" s="22">
+        <v>24.473600000000001</v>
+      </c>
+      <c r="AL50" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM50" s="20">
+        <v>552.18100000000004</v>
+      </c>
+      <c r="AN50" s="21">
+        <f>(AM50-$D50)</f>
+        <v>323.57810000000006</v>
+      </c>
+      <c r="AO50" s="22">
+        <v>3.6674199999999999</v>
+      </c>
+      <c r="AT50" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU50" s="20">
+        <v>359.59800000000001</v>
+      </c>
+      <c r="AV50" s="21">
+        <f>(AU50-$D50)</f>
+        <v>130.99510000000001</v>
+      </c>
+      <c r="AW50" s="22">
+        <v>50.215000000000003</v>
+      </c>
+      <c r="BB50" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="BC50" s="20">
+        <v>367.45800000000003</v>
+      </c>
+      <c r="BD50" s="21">
+        <f>(BC50-$D50)</f>
+        <v>138.85510000000002</v>
+      </c>
+      <c r="BE50" s="22">
+        <v>3.4799500000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:57" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="18" t="s">
         <v>57</v>
       </c>
@@ -4579,8 +7339,60 @@
       <c r="Y51" s="22">
         <v>5.9168400000000003E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD51" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE51" s="20">
+        <v>560.053</v>
+      </c>
+      <c r="AF51" s="21">
+        <f>(AE51-$D51)</f>
+        <v>333.30766000000096</v>
+      </c>
+      <c r="AG51" s="22">
+        <v>24.600100000000001</v>
+      </c>
+      <c r="AL51" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="AM51" s="20">
+        <v>509.5</v>
+      </c>
+      <c r="AN51" s="21">
+        <f>(AM51-$D51)</f>
+        <v>282.75466000000097</v>
+      </c>
+      <c r="AO51" s="22">
+        <v>3.5009100000000002</v>
+      </c>
+      <c r="AT51" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="AU51" s="20">
+        <v>331.59</v>
+      </c>
+      <c r="AV51" s="21">
+        <f>(AU51-$D51)</f>
+        <v>104.84466000000097</v>
+      </c>
+      <c r="AW51" s="22">
+        <v>43.451300000000003</v>
+      </c>
+      <c r="BB51" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="BC51" s="20">
+        <v>324.52300000000002</v>
+      </c>
+      <c r="BD51" s="21">
+        <f>(BC51-$D51)</f>
+        <v>97.777660000001021</v>
+      </c>
+      <c r="BE51" s="22">
+        <v>3.4700799999999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:57" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
         <v>58</v>
       </c>
@@ -4632,8 +7444,60 @@
       <c r="Y52" s="22">
         <v>9.1517000000000001E-2</v>
       </c>
-    </row>
-    <row r="53" spans="1:25" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD52" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE52" s="20">
+        <v>589.82600000000002</v>
+      </c>
+      <c r="AF52" s="21">
+        <f>(AE52-$D52)</f>
+        <v>363.41638999999702</v>
+      </c>
+      <c r="AG52" s="22">
+        <v>25.227499999999999</v>
+      </c>
+      <c r="AL52" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM52" s="20">
+        <v>643.86</v>
+      </c>
+      <c r="AN52" s="21">
+        <f>(AM52-$D52)</f>
+        <v>417.45038999999701</v>
+      </c>
+      <c r="AO52" s="22">
+        <v>3.5022600000000002</v>
+      </c>
+      <c r="AT52" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU52" s="20">
+        <v>386.68200000000002</v>
+      </c>
+      <c r="AV52" s="21">
+        <f>(AU52-$D52)</f>
+        <v>160.27238999999702</v>
+      </c>
+      <c r="AW52" s="22">
+        <v>51.1753</v>
+      </c>
+      <c r="BB52" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC52" s="20">
+        <v>409.053</v>
+      </c>
+      <c r="BD52" s="21">
+        <f>(BC52-$D52)</f>
+        <v>182.643389999997</v>
+      </c>
+      <c r="BE52" s="22">
+        <v>3.4181300000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:57" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="18" t="s">
         <v>59</v>
       </c>
@@ -4685,27 +7549,126 @@
       <c r="Y53" s="22">
         <v>8.0433900000000003E-2</v>
       </c>
+      <c r="AD53" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE53" s="20">
+        <v>581.13900000000001</v>
+      </c>
+      <c r="AF53" s="21">
+        <f>(AE53-$D53)</f>
+        <v>332.28238000000204</v>
+      </c>
+      <c r="AG53" s="22">
+        <v>25.964600000000001</v>
+      </c>
+      <c r="AL53" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM53" s="20">
+        <v>560.27300000000002</v>
+      </c>
+      <c r="AN53" s="21">
+        <f>(AM53-$D53)</f>
+        <v>311.41638000000205</v>
+      </c>
+      <c r="AO53" s="22">
+        <v>3.5316800000000002</v>
+      </c>
+      <c r="AT53" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="AU53" s="20">
+        <v>304.53500000000003</v>
+      </c>
+      <c r="AV53" s="21">
+        <f>(AU53-$D53)</f>
+        <v>55.678380000002022</v>
+      </c>
+      <c r="AW53" s="22">
+        <v>52.063800000000001</v>
+      </c>
+      <c r="BB53" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="BC53" s="20">
+        <v>363.41</v>
+      </c>
+      <c r="BD53" s="21">
+        <f>(BC53-$D53)</f>
+        <v>114.55338000000202</v>
+      </c>
+      <c r="BE53" s="22">
+        <v>3.4560300000000002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:57" ht="15" x14ac:dyDescent="0.2">
+      <c r="F55" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="N55" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="V55" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD55" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL55" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="AT55" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="BB55" s="38" t="s">
+        <v>66</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <autoFilter ref="H4:H53" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <mergeCells count="3">
+  <mergeCells count="7">
+    <mergeCell ref="AL2:AO2"/>
+    <mergeCell ref="AT2:AW2"/>
+    <mergeCell ref="BB2:BE2"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AD2:AG2"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="H4:H53">
+    <cfRule type="cellIs" dxfId="8" priority="7" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P4:P53">
+    <cfRule type="cellIs" dxfId="7" priority="6" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X4:X53">
+    <cfRule type="cellIs" dxfId="6" priority="5" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF4:AF53">
+    <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN4:AN53">
     <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P4:P53">
+  <conditionalFormatting sqref="AV4:AV53">
     <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X4:X53">
+  <conditionalFormatting sqref="BD4:BD53">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
idk what has been updated in the data spreadsheet
</commit_message>
<xml_diff>
--- a/memoria/resources/Tablas_MDD_2021-22.xlsx
+++ b/memoria/resources/Tablas_MDD_2021-22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/MH/memoria/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAED7789-9794-C249-AF0E-259740CFE7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB02DB4-27CA-BF40-83BB-EDB8B9FD9535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1033,7 +1033,26 @@
         <cx:tickLabels/>
       </cx:axis>
     </cx:plotArea>
-    <cx:legend pos="r" align="ctr" overlay="0"/>
+    <cx:legend pos="r" align="ctr" overlay="0">
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:sysClr>
+            </a:solidFill>
+            <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+          </a:endParaRPr>
+        </a:p>
+      </cx:txPr>
+    </cx:legend>
   </cx:chart>
 </cx:chartSpace>
 </file>
@@ -2031,10 +2050,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DO55"/>
+  <dimension ref="A1:DP55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CG1" zoomScale="68" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="DJ52" sqref="DJ52"/>
+    <sheetView tabSelected="1" topLeftCell="CX1" zoomScale="81" zoomScaleNormal="132" workbookViewId="0">
+      <selection activeCell="DN4" sqref="DN4:DP53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2051,7 +2070,7 @@
     <col min="22" max="22" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:119" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:120" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2071,7 +2090,7 @@
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:119" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:120" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -2168,7 +2187,7 @@
       <c r="DH2" s="40"/>
       <c r="DI2" s="40"/>
     </row>
-    <row r="3" spans="1:119" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:120" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
@@ -2357,7 +2376,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:119" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:120" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>8</v>
       </c>
@@ -2560,8 +2579,9 @@
         <v>9.0347999999999996E-5</v>
       </c>
       <c r="DO4" s="34"/>
-    </row>
-    <row r="5" spans="1:119" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="DP4" s="34"/>
+    </row>
+    <row r="5" spans="1:120" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>9</v>
       </c>
@@ -2764,8 +2784,9 @@
         <v>6.5708000000000002E-5</v>
       </c>
       <c r="DO5" s="34"/>
-    </row>
-    <row r="6" spans="1:119" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="DP5" s="34"/>
+    </row>
+    <row r="6" spans="1:120" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>10</v>
       </c>
@@ -3062,8 +3083,9 @@
         <v>58.744474000000046</v>
       </c>
       <c r="DO6" s="34"/>
-    </row>
-    <row r="7" spans="1:119" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="DP6" s="34"/>
+    </row>
+    <row r="7" spans="1:120" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>12</v>
       </c>
@@ -3360,8 +3382,9 @@
         <v>0.32517362261999999</v>
       </c>
       <c r="DO7" s="34"/>
-    </row>
-    <row r="8" spans="1:119" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="DP7" s="34"/>
+    </row>
+    <row r="8" spans="1:120" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>14</v>
       </c>
@@ -3564,8 +3587,9 @@
         <v>6.5011000000000005E-5</v>
       </c>
       <c r="DO8" s="34"/>
-    </row>
-    <row r="9" spans="1:119" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="DP8" s="34"/>
+    </row>
+    <row r="9" spans="1:120" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>15</v>
       </c>
@@ -3767,8 +3791,9 @@
       <c r="DI9" s="22">
         <v>4.7758299999999997E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:119" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="DP9" s="34"/>
+    </row>
+    <row r="10" spans="1:120" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>16</v>
       </c>
@@ -3970,8 +3995,9 @@
       <c r="DI10" s="22">
         <v>4.1916299999999997E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:119" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="DP10" s="34"/>
+    </row>
+    <row r="11" spans="1:120" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>17</v>
       </c>
@@ -4173,8 +4199,9 @@
       <c r="DI11" s="22">
         <v>4.5153400000000003E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:119" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="DP11" s="34"/>
+    </row>
+    <row r="12" spans="1:120" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>18</v>
       </c>
@@ -4376,8 +4403,9 @@
       <c r="DI12" s="22">
         <v>4.2893899999999999E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:119" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="DP12" s="34"/>
+    </row>
+    <row r="13" spans="1:120" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>19</v>
       </c>
@@ -4579,8 +4607,9 @@
       <c r="DI13" s="22">
         <v>4.5690599999999998E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:119" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="DP13" s="34"/>
+    </row>
+    <row r="14" spans="1:120" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>20</v>
       </c>
@@ -4782,8 +4811,9 @@
       <c r="DI14" s="22">
         <v>0.11716500000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:119" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="DP14" s="34"/>
+    </row>
+    <row r="15" spans="1:120" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>21</v>
       </c>
@@ -4985,8 +5015,9 @@
       <c r="DI15" s="22">
         <v>0.121752</v>
       </c>
-    </row>
-    <row r="16" spans="1:119" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="DP15" s="34"/>
+    </row>
+    <row r="16" spans="1:120" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>22</v>
       </c>
@@ -5188,8 +5219,9 @@
       <c r="DI16" s="22">
         <v>0.112414</v>
       </c>
-    </row>
-    <row r="17" spans="1:113" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="DP16" s="34"/>
+    </row>
+    <row r="17" spans="1:120" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>23</v>
       </c>
@@ -5391,8 +5423,9 @@
       <c r="DI17" s="22">
         <v>0.118128</v>
       </c>
-    </row>
-    <row r="18" spans="1:113" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="DP17" s="34"/>
+    </row>
+    <row r="18" spans="1:120" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>24</v>
       </c>
@@ -5594,8 +5627,9 @@
       <c r="DI18" s="22">
         <v>0.116231</v>
       </c>
-    </row>
-    <row r="19" spans="1:113" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="DP18" s="34"/>
+    </row>
+    <row r="19" spans="1:120" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>25</v>
       </c>
@@ -5798,7 +5832,7 @@
         <v>0.19076699999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:113" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:120" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>26</v>
       </c>
@@ -6001,7 +6035,7 @@
         <v>0.18231900000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:113" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:120" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>27</v>
       </c>
@@ -6204,7 +6238,7 @@
         <v>0.187803</v>
       </c>
     </row>
-    <row r="22" spans="1:113" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:120" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
         <v>28</v>
       </c>
@@ -6407,7 +6441,7 @@
         <v>0.188615</v>
       </c>
     </row>
-    <row r="23" spans="1:113" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:120" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>29</v>
       </c>
@@ -6610,7 +6644,7 @@
         <v>0.193413</v>
       </c>
     </row>
-    <row r="24" spans="1:113" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:120" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
         <v>30</v>
       </c>
@@ -6813,7 +6847,7 @@
         <v>0.30216199999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:113" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:120" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>31</v>
       </c>
@@ -7010,7 +7044,7 @@
         <v>0.31004199999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:113" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:120" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
         <v>32</v>
       </c>
@@ -7207,7 +7241,7 @@
         <v>0.31945499999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:113" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:120" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
         <v>33</v>
       </c>
@@ -7404,7 +7438,7 @@
         <v>0.32272000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:113" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:120" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>34</v>
       </c>
@@ -7601,7 +7635,7 @@
         <v>0.32359199999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:113" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:120" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>35</v>
       </c>
@@ -7798,7 +7832,7 @@
         <v>0.47226400000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:113" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:120" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>36</v>
       </c>
@@ -8001,7 +8035,7 @@
         <v>0.48450599999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:113" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:120" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
         <v>37</v>
       </c>
@@ -8198,7 +8232,7 @@
         <v>0.51142699999999996</v>
       </c>
     </row>
-    <row r="32" spans="1:113" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:120" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
improve box and whisker diagram readability
</commit_message>
<xml_diff>
--- a/memoria/resources/Tablas_MDD_2021-22.xlsx
+++ b/memoria/resources/Tablas_MDD_2021-22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/MH/memoria/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3DDCC54-EDDC-A043-82DC-D838EE5BCDD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA06FAA0-47B0-034F-BBB9-BA666991FE5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,21 @@
     <definedName name="_xlchart.v1.4" hidden="1">'2021-22'!$BK$4:$BK$53</definedName>
     <definedName name="_xlchart.v1.40" hidden="1">'2021-22'!$O$4:$O$53</definedName>
     <definedName name="_xlchart.v1.41" hidden="1">'2021-22'!$W$4:$W$53</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">'2021-22'!$AE$4:$AE$53</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">'2021-22'!$AM$4:$AM$53</definedName>
+    <definedName name="_xlchart.v1.44" hidden="1">'2021-22'!$AU$4:$AU$53</definedName>
+    <definedName name="_xlchart.v1.45" hidden="1">'2021-22'!$BC$4:$BC$53</definedName>
+    <definedName name="_xlchart.v1.46" hidden="1">'2021-22'!$BK$4:$BK$53</definedName>
+    <definedName name="_xlchart.v1.47" hidden="1">'2021-22'!$BS$4:$BS$53</definedName>
+    <definedName name="_xlchart.v1.48" hidden="1">'2021-22'!$CA$4:$CA$53</definedName>
+    <definedName name="_xlchart.v1.49" hidden="1">'2021-22'!$CI$4:$CI$53</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">'2021-22'!$BS$4:$BS$53</definedName>
+    <definedName name="_xlchart.v1.50" hidden="1">'2021-22'!$CQ$4:$CQ$53</definedName>
+    <definedName name="_xlchart.v1.51" hidden="1">'2021-22'!$CY$4:$CY$53</definedName>
+    <definedName name="_xlchart.v1.52" hidden="1">'2021-22'!$DG$4:$DG$53</definedName>
+    <definedName name="_xlchart.v1.53" hidden="1">'2021-22'!$G$4:$G$53</definedName>
+    <definedName name="_xlchart.v1.54" hidden="1">'2021-22'!$O$4:$O$53</definedName>
+    <definedName name="_xlchart.v1.55" hidden="1">'2021-22'!$W$4:$W$53</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">'2021-22'!$CA$4:$CA$53</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">'2021-22'!$CI$4:$CI$53</definedName>
     <definedName name="_xlchart.v1.8" hidden="1">'2021-22'!$CQ$4:$CQ$53</definedName>
@@ -879,72 +893,72 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.25</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.26</cx:f>
+        <cx:f>_xlchart.v1.12</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.27</cx:f>
+        <cx:f>_xlchart.v1.13</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.14</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.15</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="5">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.16</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="6">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.17</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="7">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.18</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="8">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.19</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="9">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.20</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="10">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.21</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="11">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.22</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="12">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.23</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="13">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.24</cx:f>
+        <cx:f>_xlchart.v1.10</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1274,8 +1288,42 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="18">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
   <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
 </cs:colorStyle>
 </file>
 
@@ -2235,7 +2283,7 @@
   <dimension ref="A1:DP55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E45" zoomScale="91" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="R74" sqref="R74"/>
+      <selection activeCell="R73" sqref="R73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>